<commit_message>
feat: added new features!! now, code translate to english texts using googletranslate!!
</commit_message>
<xml_diff>
--- a/Palabras_Crypto.xlsx
+++ b/Palabras_Crypto.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>PALABRAS</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>eur</t>
+  </si>
+  <si>
+    <t>ath</t>
+  </si>
+  <si>
+    <t>whale</t>
+  </si>
+  <si>
+    <t>ballena</t>
+  </si>
+  <si>
+    <t>nft</t>
   </si>
 </sst>
 </file>
@@ -225,17 +237,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.1989795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,6 +648,26 @@
       <c r="C31" s="0" t="str">
         <f aca="false">CONCATENATE("$", A31)</f>
         <v>$eur</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>